<commit_message>
Updated test data for DC,TripCurrent, Voltdrop,BatteryStandby
</commit_message>
<xml_diff>
--- a/Test Data/TC_148_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_Slot_Cards.xlsx
+++ b/Test Data/TC_148_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_Slot_Cards.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E2F242-0A62-4F6B-9551-F6BE92DE1F71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1B3322-1161-4630-8AAB-FFE458D00D43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,9 +130,6 @@
     <t xml:space="preserve">                                           Panel Accessories</t>
   </si>
   <si>
-    <t>IOB800</t>
-  </si>
-  <si>
     <t xml:space="preserve">Accessories </t>
   </si>
   <si>
@@ -157,7 +154,10 @@
     <t>NGC-488/T395 OR TC-148</t>
   </si>
   <si>
-    <t>IOB800 - 1</t>
+    <t>POS800-M - 1</t>
+  </si>
+  <si>
+    <t>POS800-M</t>
   </si>
 </sst>
 </file>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -726,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="22"/>
@@ -846,10 +846,10 @@
         <v>27</v>
       </c>
       <c r="S7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -876,13 +876,13 @@
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L8" s="7">
         <v>1.7000000000000001E-2</v>
@@ -891,25 +891,25 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="N8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="P8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q8" s="7">
-        <v>2.9000000000000001E-2</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="R8" s="7">
-        <v>0.20799999999999999</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="S8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>